<commit_message>
*Changes to static urls (implementation of dynamic parts of the personal space ID from LoginData.xslx *Optimization of CreateAccount() method in Base.java *Integration of Cucumber into TestNg framework
</commit_message>
<xml_diff>
--- a/src/main/java/resources/LoginData.xlsx
+++ b/src/main/java/resources/LoginData.xlsx
@@ -11,19 +11,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>yourmail@mail.com</t>
   </si>
   <si>
     <t>YourPassword</t>
   </si>
+  <si>
+    <t>https://d5e0000019ce6eai</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -31,6 +34,12 @@
     </font>
     <font>
       <sz val="8.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -52,7 +61,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -62,13 +71,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -298,46 +310,51 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
*Dynamic environment url implementation *Code cleaning and optimization regarding driver object
</commit_message>
<xml_diff>
--- a/src/main/java/resources/LoginData.xlsx
+++ b/src/main/java/resources/LoginData.xlsx
@@ -11,22 +11,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>yourmail@mail.com</t>
   </si>
   <si>
     <t>YourPassword</t>
   </si>
-  <si>
-    <t>https://d5e0000019ce6eai</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -34,12 +31,6 @@
     </font>
     <font>
       <sz val="8.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8.0"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -61,7 +52,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -71,16 +62,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -310,51 +298,46 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="3"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="C1"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>